<commit_message>
Updated DC Metro Data (Bus and Rail)
</commit_message>
<xml_diff>
--- a/dc_data/DCBudgetMetroBusOrignal.xlsx
+++ b/dc_data/DCBudgetMetroBusOrignal.xlsx
@@ -26,45 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Budget </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coverage </t>
-  </si>
-  <si>
-    <t>Population</t>
-  </si>
-  <si>
-    <t>2012_01</t>
-  </si>
-  <si>
-    <t>2012_02</t>
-  </si>
-  <si>
-    <t>2012_03</t>
-  </si>
-  <si>
-    <t>2012_04</t>
-  </si>
-  <si>
-    <t>2012_05</t>
-  </si>
-  <si>
-    <t>2012_06</t>
-  </si>
-  <si>
-    <t>2012_07</t>
-  </si>
-  <si>
-    <t>2012_08</t>
-  </si>
-  <si>
-    <t>2012_09</t>
-  </si>
-  <si>
     <t>2012_10</t>
   </si>
   <si>
@@ -74,36 +35,6 @@
     <t>2012_12</t>
   </si>
   <si>
-    <t>Performance (in millions)</t>
-  </si>
-  <si>
-    <t>2010_01</t>
-  </si>
-  <si>
-    <t>2010_02</t>
-  </si>
-  <si>
-    <t>2010_03</t>
-  </si>
-  <si>
-    <t>2010_04</t>
-  </si>
-  <si>
-    <t>2010_05</t>
-  </si>
-  <si>
-    <t>2010_06</t>
-  </si>
-  <si>
-    <t>2010_07</t>
-  </si>
-  <si>
-    <t>2010_08</t>
-  </si>
-  <si>
-    <t>2010_09</t>
-  </si>
-  <si>
     <t>2010_10</t>
   </si>
   <si>
@@ -113,33 +44,6 @@
     <t>2010_12</t>
   </si>
   <si>
-    <t>2011_01</t>
-  </si>
-  <si>
-    <t>2011_02</t>
-  </si>
-  <si>
-    <t>2011_03</t>
-  </si>
-  <si>
-    <t>2011_04</t>
-  </si>
-  <si>
-    <t>2011_05</t>
-  </si>
-  <si>
-    <t>2011_06</t>
-  </si>
-  <si>
-    <t>2011_07</t>
-  </si>
-  <si>
-    <t>2011_08</t>
-  </si>
-  <si>
-    <t>2011_09</t>
-  </si>
-  <si>
     <t>2011_10</t>
   </si>
   <si>
@@ -149,33 +53,6 @@
     <t>2011_12</t>
   </si>
   <si>
-    <t>2013_01</t>
-  </si>
-  <si>
-    <t>2013_02</t>
-  </si>
-  <si>
-    <t>2013_03</t>
-  </si>
-  <si>
-    <t>2013_04</t>
-  </si>
-  <si>
-    <t>2013_05</t>
-  </si>
-  <si>
-    <t>2013_06</t>
-  </si>
-  <si>
-    <t>2013_07</t>
-  </si>
-  <si>
-    <t>2013_08</t>
-  </si>
-  <si>
-    <t>2013_09</t>
-  </si>
-  <si>
     <t>2013_10</t>
   </si>
   <si>
@@ -185,33 +62,6 @@
     <t>2013_12</t>
   </si>
   <si>
-    <t>2014_01</t>
-  </si>
-  <si>
-    <t>2014_02</t>
-  </si>
-  <si>
-    <t>2014_03</t>
-  </si>
-  <si>
-    <t>2014_04</t>
-  </si>
-  <si>
-    <t>2014_05</t>
-  </si>
-  <si>
-    <t>2014_06</t>
-  </si>
-  <si>
-    <t>2014_07</t>
-  </si>
-  <si>
-    <t>2014_08</t>
-  </si>
-  <si>
-    <t>2014_09</t>
-  </si>
-  <si>
     <t>2014_10</t>
   </si>
   <si>
@@ -221,33 +71,6 @@
     <t>2014_12</t>
   </si>
   <si>
-    <t>2009_01</t>
-  </si>
-  <si>
-    <t>2009_02</t>
-  </si>
-  <si>
-    <t>2009_03</t>
-  </si>
-  <si>
-    <t>2009_04</t>
-  </si>
-  <si>
-    <t>2009_05</t>
-  </si>
-  <si>
-    <t>2009_06</t>
-  </si>
-  <si>
-    <t>2009_07</t>
-  </si>
-  <si>
-    <t>2009_08</t>
-  </si>
-  <si>
-    <t>2009_09</t>
-  </si>
-  <si>
     <t>2009_10</t>
   </si>
   <si>
@@ -255,6 +78,183 @@
   </si>
   <si>
     <t>2009_12</t>
+  </si>
+  <si>
+    <t>2009_1</t>
+  </si>
+  <si>
+    <t>2009_2</t>
+  </si>
+  <si>
+    <t>2009_3</t>
+  </si>
+  <si>
+    <t>2009_4</t>
+  </si>
+  <si>
+    <t>2009_5</t>
+  </si>
+  <si>
+    <t>2009_6</t>
+  </si>
+  <si>
+    <t>2009_7</t>
+  </si>
+  <si>
+    <t>2009_8</t>
+  </si>
+  <si>
+    <t>2009_9</t>
+  </si>
+  <si>
+    <t>2010_1</t>
+  </si>
+  <si>
+    <t>2010_2</t>
+  </si>
+  <si>
+    <t>2010_3</t>
+  </si>
+  <si>
+    <t>2010_4</t>
+  </si>
+  <si>
+    <t>2010_5</t>
+  </si>
+  <si>
+    <t>2010_6</t>
+  </si>
+  <si>
+    <t>2010_7</t>
+  </si>
+  <si>
+    <t>2010_8</t>
+  </si>
+  <si>
+    <t>2010_9</t>
+  </si>
+  <si>
+    <t>2011_1</t>
+  </si>
+  <si>
+    <t>2011_2</t>
+  </si>
+  <si>
+    <t>2011_3</t>
+  </si>
+  <si>
+    <t>2011_4</t>
+  </si>
+  <si>
+    <t>2011_5</t>
+  </si>
+  <si>
+    <t>2011_6</t>
+  </si>
+  <si>
+    <t>2011_7</t>
+  </si>
+  <si>
+    <t>2011_8</t>
+  </si>
+  <si>
+    <t>2011_9</t>
+  </si>
+  <si>
+    <t>2012_1</t>
+  </si>
+  <si>
+    <t>2012_2</t>
+  </si>
+  <si>
+    <t>2012_3</t>
+  </si>
+  <si>
+    <t>2012_4</t>
+  </si>
+  <si>
+    <t>2012_5</t>
+  </si>
+  <si>
+    <t>2012_6</t>
+  </si>
+  <si>
+    <t>2012_7</t>
+  </si>
+  <si>
+    <t>2012_8</t>
+  </si>
+  <si>
+    <t>2012_9</t>
+  </si>
+  <si>
+    <t>2013_1</t>
+  </si>
+  <si>
+    <t>2013_2</t>
+  </si>
+  <si>
+    <t>2013_3</t>
+  </si>
+  <si>
+    <t>2013_4</t>
+  </si>
+  <si>
+    <t>2013_5</t>
+  </si>
+  <si>
+    <t>2013_6</t>
+  </si>
+  <si>
+    <t>2013_7</t>
+  </si>
+  <si>
+    <t>2013_8</t>
+  </si>
+  <si>
+    <t>2013_9</t>
+  </si>
+  <si>
+    <t>2014_1</t>
+  </si>
+  <si>
+    <t>2014_2</t>
+  </si>
+  <si>
+    <t>2014_3</t>
+  </si>
+  <si>
+    <t>2014_4</t>
+  </si>
+  <si>
+    <t>2014_5</t>
+  </si>
+  <si>
+    <t>2014_6</t>
+  </si>
+  <si>
+    <t>2014_7</t>
+  </si>
+  <si>
+    <t>2014_8</t>
+  </si>
+  <si>
+    <t>2014_9</t>
+  </si>
+  <si>
+    <t>RIDERSHIP</t>
+  </si>
+  <si>
+    <t>YEAR-MONTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUDGET </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COVERAGE </t>
+  </si>
+  <si>
+    <t>POPULATION</t>
   </si>
 </sst>
 </file>
@@ -609,31 +609,38 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>12100000</v>
@@ -647,7 +654,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>11700000</v>
@@ -661,7 +668,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>11900000</v>
@@ -675,7 +682,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>12300000</v>
@@ -689,7 +696,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>10200000</v>
@@ -703,7 +710,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>10500000</v>
@@ -717,7 +724,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>10200000</v>
@@ -731,7 +738,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>10200000</v>
@@ -745,7 +752,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>11300000</v>
@@ -759,7 +766,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>11200000</v>
@@ -773,7 +780,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>10900000</v>
@@ -787,7 +794,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>11300000</v>
@@ -801,7 +808,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>11800000</v>
@@ -815,7 +822,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>11200000</v>
@@ -829,7 +836,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>11400000</v>
@@ -843,7 +850,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>11300000</v>
@@ -857,7 +864,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>9800000</v>
@@ -871,7 +878,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>9300000</v>
@@ -885,7 +892,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>9600000</v>
@@ -899,7 +906,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>7100000</v>
@@ -913,7 +920,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B22">
         <v>11000000</v>
@@ -927,7 +934,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B23">
         <v>10800000</v>
@@ -941,7 +948,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B24">
         <v>10300000</v>
@@ -955,7 +962,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>10500000</v>
@@ -969,7 +976,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>16000000</v>
@@ -983,7 +990,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>16000000</v>
@@ -997,7 +1004,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>19700000</v>
@@ -1011,7 +1018,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>19300000</v>
@@ -1025,7 +1032,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>18400000</v>
@@ -1039,7 +1046,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B31">
         <v>20000000</v>
@@ -1053,7 +1060,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>19500000</v>
@@ -1067,7 +1074,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <v>18400000</v>
@@ -1081,7 +1088,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>18000000</v>
@@ -1095,7 +1102,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B35">
         <v>18500000</v>
@@ -1109,7 +1116,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B36">
         <v>17200000</v>
@@ -1123,7 +1130,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B37">
         <v>16400000</v>
@@ -1137,7 +1144,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B38">
         <v>10800000</v>
@@ -1151,7 +1158,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B39">
         <v>10900000</v>
@@ -1165,7 +1172,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B40">
         <v>11700000</v>
@@ -1179,7 +1186,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="B41">
         <v>11000000</v>
@@ -1193,7 +1200,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="B42">
         <v>11600000</v>
@@ -1207,7 +1214,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B43">
         <v>11000000</v>
@@ -1221,7 +1228,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="B44">
         <v>11200000</v>
@@ -1235,7 +1242,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B45">
         <v>11900000</v>
@@ -1249,7 +1256,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B46">
         <v>11300000</v>
@@ -1263,7 +1270,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B47">
         <v>11200000</v>
@@ -1277,7 +1284,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B48">
         <v>10800000</v>
@@ -1291,7 +1298,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B49">
         <v>10100000</v>
@@ -1305,7 +1312,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B50">
         <v>10700000</v>
@@ -1319,7 +1326,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B51">
         <v>10400000</v>
@@ -1333,7 +1340,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B52">
         <v>11300000</v>
@@ -1347,7 +1354,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B53">
         <v>11600000</v>
@@ -1361,7 +1368,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B54">
         <v>12100000</v>
@@ -1375,7 +1382,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B55">
         <v>11200000</v>
@@ -1389,7 +1396,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B56">
         <v>11800000</v>
@@ -1403,7 +1410,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B57">
         <v>11700000</v>
@@ -1417,7 +1424,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B58">
         <v>11700000</v>
@@ -1431,7 +1438,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B59">
         <v>12300000</v>
@@ -1445,7 +1452,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="B60">
         <v>11000000</v>
@@ -1459,7 +1466,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="B61">
         <v>10400000</v>
@@ -1473,7 +1480,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B62">
         <v>10500000</v>
@@ -1487,7 +1494,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B63">
         <v>10100000</v>
@@ -1501,7 +1508,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>10800000</v>
@@ -1515,7 +1522,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <v>11800000</v>
@@ -1529,7 +1536,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <v>11800000</v>
@@ -1543,7 +1550,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>11600000</v>
@@ -1557,7 +1564,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B68">
         <v>11900000</v>
@@ -1571,7 +1578,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B69">
         <v>11600000</v>
@@ -1585,7 +1592,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B70">
         <v>11900000</v>
@@ -1599,7 +1606,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="B71">
         <v>12300000</v>
@@ -1613,7 +1620,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="B72">
         <v>10200000</v>
@@ -1627,7 +1634,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="B73">
         <v>10500000</v>

</xml_diff>